<commit_message>
Updated Baseline and FollowUp
</commit_message>
<xml_diff>
--- a/Data/ChildCareEC.xlsx
+++ b/Data/ChildCareEC.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -15,10 +15,18 @@
   <sheets>
     <sheet name="Question Bank " sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028" concurrentCalc="0"/>
+  <calcPr calcId="191028" calcCompleted="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -30,10 +38,10 @@
     <t>Question</t>
   </si>
   <si>
-    <t>Current</t>
-  </si>
-  <si>
-    <t>Past</t>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Occurrence</t>
   </si>
   <si>
     <t xml:space="preserve">Prior to the coronavirus (COVID-19) Pandemic, did you use any non-parental care for your child(ren) under the age of 5? 
@@ -42,18 +50,21 @@
 • Unsure </t>
   </si>
   <si>
+    <t>Current</t>
+  </si>
+  <si>
     <t xml:space="preserve">This week, have you used any non-parental care for your child(ren) under the age of 5?  
 • Yes 
 • No 
 • Unsure </t>
   </si>
   <si>
-    <t xml:space="preserve">Do you expect your need for non-parental care for your child under the age of 5 to change in the next month?  
-• Yes, I will need more non-parental care 
-• Yes, I will need less non-parental care  
-• Maybe I will need more non-parental care   
-• Maybe I will need less non-parental care   
-• No, I expect to have the same need for non-parental care 
+    <t xml:space="preserve">Do you expect your need for non-parental care for your child under the age of 5 to change in the next month?  _x000D_
+• Yes, I will need more non-parental care _x000D_
+• Yes, I will need less non-parental care  _x000D_
+• Maybe I will need more non-parental care   _x000D_
+• Maybe I will need less non-parental care   _x000D_
+• No, I expect to have the same need for non-parental care _x000D_
 • Not Applicable </t>
   </si>
   <si>
@@ -65,6 +76,9 @@
 • At least five hours of paid care by a professional child care provider in their home   
 • Care provided entirely by the child’s parents and/or legal guardians   
 • None of the above apply   </t>
+  </si>
+  <si>
+    <t>Past</t>
   </si>
   <si>
     <t xml:space="preserve">In a typical week, before the coronavirus (COVID-19) pandemic, which of the following types of childcare did you use for your child(ren) in the age range 0-5? Select all that apply. 
@@ -405,12 +419,6 @@
   </si>
   <si>
     <t>With respect to your worries, concerns, or challenges for your children, what has or would help to alleviate these issues or make things better?</t>
-  </si>
-  <si>
-    <t>Source</t>
-  </si>
-  <si>
-    <t>Occurrence</t>
   </si>
 </sst>
 </file>
@@ -776,10 +784,10 @@
   <dimension ref="A1:C50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
   <cols>
     <col min="1" max="1" width="75" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
@@ -791,451 +799,451 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="85">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="84.95">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="68">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="68.099999999999994">
       <c r="A3" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="136">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="126">
       <c r="A4" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="204">
       <c r="A5" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="221">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="221.1">
       <c r="A6" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="51">
       <c r="A7" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="153">
       <c r="A8" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="204">
       <c r="A9" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="187">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="186.95">
       <c r="A10" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="136">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="135.94999999999999">
       <c r="A11" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="34">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="33.950000000000003">
       <c r="A12" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="153">
       <c r="A13" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="136">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="135.94999999999999">
       <c r="A14" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="68">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="68.099999999999994">
       <c r="A15" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="238">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="237.95">
       <c r="A16" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="51">
       <c r="A17" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="68">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="68.099999999999994">
       <c r="A18" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="221">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="221.1">
       <c r="A19" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="34">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="33.950000000000003">
       <c r="A20" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="51">
       <c r="A21" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="102">
       <c r="A22" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="187">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="186.95">
       <c r="A23" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="153">
       <c r="A24" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="136">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="135.94999999999999">
       <c r="A25" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="102">
       <c r="A26" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="102">
       <c r="A27" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="119">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="119.1">
       <c r="A28" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="136">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="135.94999999999999">
       <c r="A29" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="204">
       <c r="A30" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="102">
       <c r="A31" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B31" s="1"/>
       <c r="C31" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="68">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="68.099999999999994">
       <c r="A32" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B32" s="1"/>
       <c r="C32" s="1" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="153">
       <c r="A33" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B33" s="1"/>
       <c r="C33" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="85">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="84.95">
       <c r="A34" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B34" s="1"/>
       <c r="C34" s="1" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="153">
       <c r="A35" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B35" s="1"/>
       <c r="C35" s="1" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="51">
       <c r="A36" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="221">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="221.1">
       <c r="A37" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B37" s="1"/>
       <c r="C37" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="221">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="221.1">
       <c r="A38" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B38" s="1"/>
       <c r="C38" s="1" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="51">
       <c r="A39" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B39" s="1"/>
       <c r="C39" s="1" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="51">
       <c r="A40" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B40" s="1"/>
       <c r="C40" s="1" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="51">
       <c r="A41" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B41" s="1"/>
       <c r="C41" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="119">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="119.1">
       <c r="A42" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B42" s="1"/>
       <c r="C42" s="1" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="102">
       <c r="A43" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B43" s="1"/>
       <c r="C43" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="187">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="186.95">
       <c r="A44" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B44" s="1"/>
       <c r="C44" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="170">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="170.1">
       <c r="A45" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B45" s="1"/>
       <c r="C45" s="1" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="204">
       <c r="A46" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B46" s="1"/>
       <c r="C46" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="119">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="119.1">
       <c r="A47" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B47" s="1"/>
       <c r="C47" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" ht="34">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="33.950000000000003">
       <c r="A48" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B48" s="1"/>
       <c r="C48" s="1" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="51">
       <c r="A49" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B49" s="1"/>
       <c r="C49" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" ht="34">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="33.950000000000003">
       <c r="A50" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B50" s="1"/>
       <c r="C50" s="1" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>